<commit_message>
Modified:Method To Handle Exception If = is not present in locator
</commit_message>
<xml_diff>
--- a/KeywordDriven/Excel File/first_keysheet.xlsx
+++ b/KeywordDriven/Excel File/first_keysheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhib\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhib\source\repos\KeywordDriven\KeywordDriven\Excel File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16BB86CD-F74C-4E29-A658-EE8088F3C2D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07D7914-5436-4C5E-9AF0-1C1CFA623E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBF446DD-EF0C-4514-9080-F701AEDA9CBC}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added:Test Case For Facebook Login
</commit_message>
<xml_diff>
--- a/KeywordDriven/Excel File/first_keysheet.xlsx
+++ b/KeywordDriven/Excel File/first_keysheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhib\source\repos\KeywordDriven\KeywordDriven\Excel File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4AF169-D8E0-47A8-B8A4-7676FE5A6271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3D9757-9430-4BAF-95A1-FE49C200FDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FBF446DD-EF0C-4514-9080-F701AEDA9CBC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Test Step</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>id=email</t>
-  </si>
-  <si>
-    <t>enfield</t>
   </si>
 </sst>
 </file>
@@ -553,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17859DAF-30E4-4476-A090-B4CF11C34321}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,107 +635,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="9" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{F14D0577-657D-422B-A298-B93CFA3854BB}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{A16C1B65-3A5E-4D54-A464-5F2552901E44}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{8C59B86B-1FCB-4032-8C73-1B9C1293E7C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020085D7-E638-43E9-BE8D-4AAFB8A4B052}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -788,126 +700,69 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>28</v>
+      <c r="D4" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6">
-        <v>9028809305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{42B99F0C-F83B-4BB0-9680-BB516D62D922}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{C2D5FD02-5394-4313-A718-ED4BA029F053}"/>
-    <hyperlink ref="D8" r:id="rId3" display="rishibodake20@gmail.com" xr:uid="{62974EE8-18B6-4316-B679-3D81D37E9713}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{A16C1B65-3A5E-4D54-A464-5F2552901E44}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{8C59B86B-1FCB-4032-8C73-1B9C1293E7C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>